<commit_message>
Changed the folder structure
</commit_message>
<xml_diff>
--- a/docs/Team.xlsx
+++ b/docs/Team.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Folder\Galal\Courses\Digital Egypt Pioneers Initiative (DEPI) - Software Testing\DEPI Software Tester Graduation Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Folder\Galal\Courses\Digital Egypt Pioneers Initiative (DEPI) - Software Testing\DEPI Software Tester Graduation Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1779FD3E-C139-4786-94C1-0F1B5C5258DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A5385C-BEF6-4F54-AECF-569786D194FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>BNS2_SWD6_S1</t>
   </si>
@@ -72,7 +72,16 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Leader</t>
+    <t>Tester, focusing on UI automation and functional testing</t>
+  </si>
+  <si>
+    <t>Tester, specializing in API testing and integration validation</t>
+  </si>
+  <si>
+    <t>Tester, handling performance testing and optimization</t>
+  </si>
+  <si>
+    <t>Scrum Master &amp; Team Lead, responsible for coordination and removing blockers</t>
   </si>
 </sst>
 </file>
@@ -596,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +616,7 @@
     <col min="3" max="3" width="21.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.88671875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -630,7 +639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>312294021</v>
       </c>
@@ -646,8 +655,8 @@
       <c r="E2" s="7">
         <v>1022546004</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -666,7 +675,9 @@
       <c r="E3" s="7">
         <v>1159356801</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
@@ -684,7 +695,9 @@
       <c r="E4" s="7">
         <v>1110939360</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
@@ -702,7 +715,9 @@
       <c r="E5" s="7">
         <v>1104723206</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">

</xml_diff>